<commit_message>
import wizard has been added
</commit_message>
<xml_diff>
--- a/Abyari/uploads/aaa.xlsx
+++ b/Abyari/uploads/aaa.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="525" windowWidth="19440" windowHeight="9525" tabRatio="614"/>
+    <workbookView xWindow="480" yWindow="525" windowWidth="19440" windowHeight="9525" tabRatio="913"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="40" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet3!$1:$309</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet3!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -2245,9 +2245,11 @@
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="6"/>
-    <col min="10" max="10" width="13.42578125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
     <col min="13" max="13" width="14.7109375" customWidth="1"/>
     <col min="14" max="14" width="11.85546875" customWidth="1"/>

</xml_diff>